<commit_message>
Finalización de Interfaz Intermedia
</commit_message>
<xml_diff>
--- a/Software Comparador/Clientes/Clientes.xlsx
+++ b/Software Comparador/Clientes/Clientes.xlsx
@@ -1,95 +1,77 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
-  <workbookProtection/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+  <workbookPr/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\micro\Projects\ComparadorLCM\Software Comparador\Clientes\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC685AB8-E186-442A-ACAC-F68C81CF3796}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="-20610" yWindow="6345" windowWidth="20730" windowHeight="11040" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId3"/>
+    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.0001"/>
-  <extLst>
-    <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="ExcelA1"/>
-    </ext>
-  </extLst>
+  <calcPr calcId="0"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
-    <t xml:space="preserve">Información Clientes</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nombre del cliente</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Contacto del cliente</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Nombre del archivo del cliente</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Instituto Costarricense de Electricidad</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Laboratoro de Dimensional del ICE, Plantel ICE en Colima, Tibás, San José, Costa Rica</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Instituto Costarricense de Electricidad.xlsx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Laboratorio de Metrología TEC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Tecnológico de Costa Rica</t>
-  </si>
-  <si>
-    <t xml:space="preserve">TEC.xlsx</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Javier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Casa de Javier</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Javier.xlsx</t>
+    <t>Información Clientes</t>
+  </si>
+  <si>
+    <t>Nombre del cliente</t>
+  </si>
+  <si>
+    <t>Contacto del cliente</t>
+  </si>
+  <si>
+    <t>Nombre del archivo del cliente</t>
+  </si>
+  <si>
+    <t>Instituto Costarricense de Electricidad</t>
+  </si>
+  <si>
+    <t>Laboratoro de Dimensional del ICE, Plantel ICE en Colima, Tibás, San José, Costa Rica</t>
+  </si>
+  <si>
+    <t>Instituto Costarricense de Electricidad.xlsx</t>
+  </si>
+  <si>
+    <t>Laboratorio de Metrología TEC</t>
+  </si>
+  <si>
+    <t>Tecnológico de Costa Rica</t>
+  </si>
+  <si>
+    <t>TEC.xlsx</t>
+  </si>
+  <si>
+    <t>Javier</t>
+  </si>
+  <si>
+    <t>Casa de Javier</t>
+  </si>
+  <si>
+    <t>Javier.xlsx</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="General"/>
-  </numFmts>
-  <fonts count="5">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
     </font>
     <font>
       <sz val="20"/>
@@ -108,128 +90,112 @@
     </fill>
   </fills>
   <borders count="2">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
       <bottom/>
       <diagonal/>
     </border>
-    <border diagonalUp="false" diagonalDown="false">
-      <left style="thin"/>
-      <right style="thin"/>
-      <top style="thin"/>
-      <bottom style="thin"/>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Tema de Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
         <a:srgbClr val="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:srgbClr val="ffffff"/>
+        <a:srgbClr val="FFFFFF"/>
       </a:lt1>
       <a:dk2>
-        <a:srgbClr val="44546a"/>
+        <a:srgbClr val="44546A"/>
       </a:dk2>
       <a:lt2>
-        <a:srgbClr val="e7e6e6"/>
+        <a:srgbClr val="E7E6E6"/>
       </a:lt2>
       <a:accent1>
-        <a:srgbClr val="4472c4"/>
+        <a:srgbClr val="4472C4"/>
       </a:accent1>
       <a:accent2>
-        <a:srgbClr val="ed7d31"/>
+        <a:srgbClr val="ED7D31"/>
       </a:accent2>
       <a:accent3>
-        <a:srgbClr val="a5a5a5"/>
+        <a:srgbClr val="A5A5A5"/>
       </a:accent3>
       <a:accent4>
-        <a:srgbClr val="ffc000"/>
+        <a:srgbClr val="FFC000"/>
       </a:accent4>
       <a:accent5>
-        <a:srgbClr val="5b9bd5"/>
+        <a:srgbClr val="5B9BD5"/>
       </a:accent5>
       <a:accent6>
-        <a:srgbClr val="70ad47"/>
+        <a:srgbClr val="70AD47"/>
       </a:accent6>
       <a:hlink>
-        <a:srgbClr val="0563c1"/>
+        <a:srgbClr val="0563C1"/>
       </a:hlink>
       <a:folHlink>
-        <a:srgbClr val="954f72"/>
+        <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204" pitchFamily="0" charset="1"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
       </a:minorFont>
@@ -261,7 +227,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
         <a:gradFill>
           <a:gsLst>
@@ -285,7 +251,7 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:fillStyleLst>
       <a:lnStyleLst>
@@ -345,52 +311,52 @@
             </a:gs>
           </a:gsLst>
           <a:lin ang="5400000" scaled="0"/>
-          <a:tileRect l="0" t="0" r="0" b="0"/>
+          <a:tileRect/>
         </a:gradFill>
       </a:bgFillStyleLst>
     </a:fmtScheme>
   </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:C8"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="132" zoomScaleNormal="132" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+    <sheetView tabSelected="1" zoomScale="132" zoomScaleNormal="132" workbookViewId="0">
+      <selection activeCell="A6" sqref="A6:C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.83203125" defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="36.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="80.83"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="40.83"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="16384" min="4" style="1" width="10.83"/>
+    <col min="1" max="1" width="36.375" style="1" customWidth="1"/>
+    <col min="2" max="2" width="80.875" style="1" customWidth="1"/>
+    <col min="3" max="3" width="40.875" style="1" customWidth="1"/>
+    <col min="4" max="4" width="10.875" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="10.875" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="24.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A1" s="2" t="s">
+    <row r="1" spans="1:3" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="2"/>
-      <c r="C1" s="2"/>
-    </row>
-    <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3" t="s">
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+    </row>
+    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="3" t="s">
+      <c r="C2" s="2" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
@@ -401,7 +367,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
         <v>7</v>
       </c>
@@ -412,30 +378,29 @@
         <v>9</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A5" s="4" t="s">
+    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="4" t="s">
+      <c r="B5" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="4" t="s">
+      <c r="C5" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="7" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
-    <row r="8" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
+    <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A6"/>
+      <c r="B6"/>
+      <c r="C6"/>
+    </row>
+    <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:C1"/>
   </mergeCells>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader/>
-    <oddFooter/>
-  </headerFooter>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Fix carga de archivos y minifix
</commit_message>
<xml_diff>
--- a/Software Comparador/Clientes/Clientes.xlsx
+++ b/Software Comparador/Clientes/Clientes.xlsx
@@ -1,62 +1,40 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27231"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Lrojas\Comparador\ComparadorLCM\Software Comparador\Clientes\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2490788F-B523-477D-A630-47BCDFBDACFE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="500" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
+    <sheet name="Hoja1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <definedNames/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
-  <si>
-    <t>Información Clientes</t>
-  </si>
-  <si>
-    <t>Nombre del cliente</t>
-  </si>
-  <si>
-    <t>Contacto del cliente</t>
-  </si>
-  <si>
-    <t>Nombre del archivo del cliente</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <numFmts count="0"/>
+  <fonts count="2">
     <font>
+      <name val="Calibri"/>
+      <charset val="1"/>
+      <family val="2"/>
+      <color theme="1"/>
       <sz val="12"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
     <font>
+      <name val="Calibri"/>
+      <charset val="1"/>
+      <family val="2"/>
+      <color theme="1"/>
       <sz val="20"/>
-      <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -90,36 +68,95 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
-      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
-    </ext>
-    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
-      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
-    </ext>
-  </extLst>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -298,62 +335,79 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C13"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="132" zoomScaleNormal="132" workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.875" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="36.375" style="1" customWidth="1"/>
-    <col min="2" max="2" width="80.875" style="1" customWidth="1"/>
-    <col min="3" max="3" width="40.875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="10.875" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="10.875" style="1"/>
+    <col width="36.375" customWidth="1" style="5" min="1" max="1"/>
+    <col width="80.875" customWidth="1" style="5" min="2" max="2"/>
+    <col width="40.875" customWidth="1" style="5" min="3" max="3"/>
+    <col width="10.875" customWidth="1" style="5" min="4" max="5"/>
+    <col width="10.875" customWidth="1" style="5" min="6" max="16384"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
+    <row r="1" ht="24.75" customHeight="1">
+      <c r="A1" s="3" t="inlineStr">
+        <is>
+          <t>Información Clientes</t>
+        </is>
+      </c>
     </row>
-    <row r="2" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>2</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>3</v>
+    <row r="2" ht="15.75" customHeight="1">
+      <c r="A2" s="2" t="inlineStr">
+        <is>
+          <t>Nombre del cliente</t>
+        </is>
+      </c>
+      <c r="B2" s="2" t="inlineStr">
+        <is>
+          <t>Contacto del cliente</t>
+        </is>
+      </c>
+      <c r="C2" s="2" t="inlineStr">
+        <is>
+          <t>Nombre del archivo del cliente</t>
+        </is>
       </c>
     </row>
-    <row r="3" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5"/>
-      <c r="B5"/>
-      <c r="C5"/>
+    <row r="3" ht="15.75" customHeight="1">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Javier</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Cartago</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>Javier.xlsx</t>
+        </is>
+      </c>
     </row>
-    <row r="6" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6"/>
-      <c r="B6"/>
-      <c r="C6"/>
+    <row r="4" ht="15.75" customHeight="1"/>
+    <row r="5" ht="15" customHeight="1">
+      <c r="C5" s="5" t="n"/>
     </row>
-    <row r="7" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="8" spans="1:3" ht="15" customHeight="1" x14ac:dyDescent="0.25"/>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="B13" s="5"/>
-    </row>
+    <row r="6" ht="15" customHeight="1"/>
+    <row r="7" ht="15" customHeight="1"/>
+    <row r="8" ht="15" customHeight="1"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:C1"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.511811023622047" footer="0.511811023622047"/>
-  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Actualizacion de codigo al dia
</commit_message>
<xml_diff>
--- a/Software Comparador/Clientes/Clientes.xlsx
+++ b/Software Comparador/Clientes/Clientes.xlsx
@@ -340,7 +340,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="132" zoomScaleNormal="132" workbookViewId="0">
       <selection activeCell="C5" sqref="C5"/>
@@ -414,9 +414,39 @@
       </c>
     </row>
     <row r="5" ht="15" customHeight="1">
-      <c r="C5" s="5" t="n"/>
-    </row>
-    <row r="6" ht="15" customHeight="1"/>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Leo</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>LCM San Pedro</t>
+        </is>
+      </c>
+      <c r="C5" s="5" t="inlineStr">
+        <is>
+          <t>Leo.xlsx</t>
+        </is>
+      </c>
+    </row>
+    <row r="6" ht="15" customHeight="1">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Instituto Costarricense de Electricidad</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>Sabana Norte edificio ICE</t>
+        </is>
+      </c>
+      <c r="C6" t="inlineStr">
+        <is>
+          <t>Instituto Costarricense de Electricidad.xlsx</t>
+        </is>
+      </c>
+    </row>
     <row r="7" ht="15" customHeight="1"/>
     <row r="8" ht="15" customHeight="1"/>
   </sheetData>

</xml_diff>